<commit_message>
Added Headers to Excel files
</commit_message>
<xml_diff>
--- a/Excel File Manual Tests/SearchResultsAgendaHTMLURLs.xlsx
+++ b/Excel File Manual Tests/SearchResultsAgendaHTMLURLs.xlsx
@@ -15,7 +15,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="175">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>AgendaHTMLiFrameURL</t>
+  </si>
+  <si>
+    <t>PageURL</t>
+  </si>
   <si>
     <t>agview.aspx?agviewmeetid=1927&amp;agviewdoctype=AGENDA</t>
   </si>
@@ -870,7 +879,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -879,949 +888,960 @@
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C55" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C60" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C61" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C62" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C63" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C65" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C70" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C71" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C74" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C75" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C76" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C77" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C78" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C81" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C82" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C83" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C84" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C85" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+      <c r="C86" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
         <v>86</v>
       </c>
-      <c r="B86" t="s">
-        <v>170</v>
-      </c>
-      <c r="C86" t="s">
-        <v>171</v>
+      <c r="B87" t="s">
+        <v>173</v>
+      </c>
+      <c r="C87" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>